<commit_message>
update excel model with accounts
</commit_message>
<xml_diff>
--- a/resources/china/Model.xlsx
+++ b/resources/china/Model.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21601"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F4A70B4-02F3-4BF2-83BA-5E30A1E3F768}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A20D219-E252-448F-96F1-803D3FF18845}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-165" yWindow="-165" windowWidth="38730" windowHeight="21930" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="info" sheetId="6" r:id="rId1"/>
@@ -15,19 +15,25 @@
     <sheet name="events" sheetId="8" r:id="rId5"/>
     <sheet name="waterfall" sheetId="2" r:id="rId6"/>
     <sheet name="assumption" sheetId="3" r:id="rId7"/>
-    <sheet name="result" sheetId="4" r:id="rId8"/>
+    <sheet name="account" sheetId="9" r:id="rId8"/>
+    <sheet name="result" sheetId="4" r:id="rId9"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="98">
   <si>
     <t>产品名称（底层）</t>
     <phoneticPr fontId="3" type="noConversion"/>
@@ -401,6 +407,30 @@
   </si>
   <si>
     <t>率</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>名称</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>类型</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>本金帐</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>利息帐</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>账户P</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>账户I</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -2879,13 +2909,13 @@
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="19.25" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="23" t="s">
         <v>25</v>
       </c>
@@ -2893,7 +2923,7 @@
         <v>42852</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="23" t="s">
         <v>26</v>
       </c>
@@ -2901,7 +2931,7 @@
         <v>42852</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="23" t="s">
         <v>27</v>
       </c>
@@ -2909,7 +2939,7 @@
         <v>42911</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="23" t="s">
         <v>28</v>
       </c>
@@ -2931,21 +2961,21 @@
       <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="11.5" customWidth="1"/>
-    <col min="2" max="2" width="15.33203125" customWidth="1"/>
-    <col min="3" max="3" width="13.33203125" customWidth="1"/>
-    <col min="4" max="4" width="14.33203125" customWidth="1"/>
-    <col min="5" max="5" width="14.08203125" customWidth="1"/>
+    <col min="2" max="2" width="15.375" customWidth="1"/>
+    <col min="3" max="3" width="13.375" customWidth="1"/>
+    <col min="4" max="4" width="14.375" customWidth="1"/>
+    <col min="5" max="5" width="14.125" customWidth="1"/>
     <col min="6" max="6" width="10.25" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.58203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="15" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.83203125" customWidth="1"/>
-    <col min="12" max="12" width="11.08203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.875" customWidth="1"/>
+    <col min="12" max="12" width="11.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="28" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" ht="27" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2983,7 +3013,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" s="6">
         <v>1</v>
       </c>
@@ -3030,7 +3060,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" s="6">
         <v>2</v>
       </c>
@@ -3077,7 +3107,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" s="6">
         <v>3</v>
       </c>
@@ -3124,7 +3154,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" s="13">
         <v>4</v>
       </c>
@@ -3171,7 +3201,7 @@
         <v>1.4986301369863013</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" s="13">
         <v>5</v>
       </c>
@@ -3233,16 +3263,16 @@
       <selection activeCell="A2" sqref="A2:A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="8" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.83203125" customWidth="1"/>
+    <col min="2" max="2" width="14.875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.875" customWidth="1"/>
     <col min="4" max="5" width="8" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.58203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="11" t="s">
         <v>16</v>
       </c>
@@ -3262,7 +3292,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="11" t="s">
         <v>21</v>
       </c>
@@ -3282,7 +3312,7 @@
         <v>43071</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="11" t="s">
         <v>22</v>
       </c>
@@ -3302,7 +3332,7 @@
         <v>44390</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="11" t="s">
         <v>23</v>
       </c>
@@ -3322,7 +3352,7 @@
         <v>44568</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="11" t="s">
         <v>24</v>
       </c>
@@ -3349,18 +3379,18 @@
       <selection activeCell="D2" sqref="D2:F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.4140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.08203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.9140625" customWidth="1"/>
-    <col min="13" max="13" width="8.08203125" customWidth="1"/>
+    <col min="1" max="1" width="14.375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.875" customWidth="1"/>
+    <col min="13" max="13" width="8.125" customWidth="1"/>
     <col min="15" max="15" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>44</v>
       </c>
@@ -3371,7 +3401,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>31</v>
       </c>
@@ -3400,7 +3430,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>41</v>
       </c>
@@ -3429,7 +3459,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>32</v>
       </c>
@@ -3459,7 +3489,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>46</v>
       </c>
@@ -3476,7 +3506,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>58</v>
       </c>
@@ -3508,19 +3538,19 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>64</v>
       </c>
@@ -3540,18 +3570,18 @@
       <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="61.4140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="61.375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="8.5" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="18.9140625" customWidth="1"/>
+    <col min="10" max="10" width="18.875" customWidth="1"/>
     <col min="11" max="11" width="14" customWidth="1"/>
     <col min="12" max="12" width="9" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="13.9140625" customWidth="1"/>
+    <col min="14" max="14" width="13.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A1" s="29" t="s">
         <v>35</v>
       </c>
@@ -3571,7 +3601,7 @@
       <c r="M1" s="29"/>
       <c r="N1" s="29"/>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>54</v>
       </c>
@@ -3612,7 +3642,7 @@
       </c>
       <c r="P2" s="26"/>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
         <v>86</v>
       </c>
@@ -3632,7 +3662,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
         <v>86</v>
       </c>
@@ -3652,7 +3682,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
         <v>86</v>
       </c>
@@ -3672,7 +3702,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
         <v>86</v>
       </c>
@@ -3698,7 +3728,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
         <v>86</v>
       </c>
@@ -3727,7 +3757,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
         <v>86</v>
       </c>
@@ -3756,7 +3786,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
         <v>86</v>
       </c>
@@ -3785,7 +3815,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
         <v>86</v>
       </c>
@@ -3814,7 +3844,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B11" t="s">
         <v>86</v>
       </c>
@@ -3840,7 +3870,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
         <v>86</v>
       </c>
@@ -3869,7 +3899,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
         <v>86</v>
       </c>
@@ -3895,7 +3925,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B14" t="s">
         <v>86</v>
       </c>
@@ -3912,7 +3942,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B15" t="s">
         <v>86</v>
       </c>
@@ -3923,7 +3953,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B16" t="s">
         <v>86</v>
       </c>
@@ -3948,13 +3978,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DAFD9C3-B9AC-49B8-BF43-4A03F520CCED}">
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>87</v>
       </c>
@@ -3962,7 +3992,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>89</v>
       </c>
@@ -3989,12 +4019,61 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4788DB3C-D649-48F4-9499-B599CC244B2F}">
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B1" t="s">
+        <v>93</v>
+      </c>
+      <c r="C1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>96</v>
+      </c>
+      <c r="B2" t="s">
+        <v>94</v>
+      </c>
+      <c r="C2">
+        <v>1200</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>97</v>
+      </c>
+      <c r="B3" t="s">
+        <v>95</v>
+      </c>
+      <c r="C3">
+        <v>300</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4ECF8EAB-26C6-4A3D-BECF-BB5BDC97EC3D}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
WIP: two new java classes
</commit_message>
<xml_diff>
--- a/resources/china/Model.xlsx
+++ b/resources/china/Model.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21601"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A20D219-E252-448F-96F1-803D3FF18845}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43DC3AC9-CD18-443C-B367-17B4D7F51986}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10350" yWindow="6315" windowWidth="13065" windowHeight="9225" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="info" sheetId="6" r:id="rId1"/>
@@ -2909,13 +2909,13 @@
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="19.25" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="23" t="s">
         <v>25</v>
       </c>
@@ -2923,7 +2923,7 @@
         <v>42852</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="23" t="s">
         <v>26</v>
       </c>
@@ -2931,7 +2931,7 @@
         <v>42852</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="23" t="s">
         <v>27</v>
       </c>
@@ -2939,7 +2939,7 @@
         <v>42911</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="23" t="s">
         <v>28</v>
       </c>
@@ -2961,21 +2961,21 @@
       <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="11.5" customWidth="1"/>
-    <col min="2" max="2" width="15.375" customWidth="1"/>
-    <col min="3" max="3" width="13.375" customWidth="1"/>
-    <col min="4" max="4" width="14.375" customWidth="1"/>
-    <col min="5" max="5" width="14.125" customWidth="1"/>
+    <col min="2" max="2" width="15.33203125" customWidth="1"/>
+    <col min="3" max="3" width="13.33203125" customWidth="1"/>
+    <col min="4" max="4" width="14.33203125" customWidth="1"/>
+    <col min="5" max="5" width="14.08203125" customWidth="1"/>
     <col min="6" max="6" width="10.25" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.58203125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="15" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.875" customWidth="1"/>
-    <col min="12" max="12" width="11.125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.83203125" customWidth="1"/>
+    <col min="12" max="12" width="11.08203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="27" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14" ht="28" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3013,7 +3013,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" s="6">
         <v>1</v>
       </c>
@@ -3060,7 +3060,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3" s="6">
         <v>2</v>
       </c>
@@ -3107,7 +3107,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A4" s="6">
         <v>3</v>
       </c>
@@ -3154,7 +3154,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A5" s="13">
         <v>4</v>
       </c>
@@ -3201,7 +3201,7 @@
         <v>1.4986301369863013</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A6" s="13">
         <v>5</v>
       </c>
@@ -3263,16 +3263,16 @@
       <selection activeCell="A2" sqref="A2:A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="8" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.875" customWidth="1"/>
+    <col min="2" max="2" width="14.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.83203125" customWidth="1"/>
     <col min="4" max="5" width="8" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.58203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="11" t="s">
         <v>16</v>
       </c>
@@ -3292,7 +3292,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="11" t="s">
         <v>21</v>
       </c>
@@ -3312,7 +3312,7 @@
         <v>43071</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="11" t="s">
         <v>22</v>
       </c>
@@ -3332,7 +3332,7 @@
         <v>44390</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="11" t="s">
         <v>23</v>
       </c>
@@ -3352,7 +3352,7 @@
         <v>44568</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="11" t="s">
         <v>24</v>
       </c>
@@ -3379,18 +3379,18 @@
       <selection activeCell="D2" sqref="D2:F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.875" customWidth="1"/>
-    <col min="13" max="13" width="8.125" customWidth="1"/>
+    <col min="1" max="1" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.08203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.83203125" customWidth="1"/>
+    <col min="13" max="13" width="8.08203125" customWidth="1"/>
     <col min="15" max="15" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>44</v>
       </c>
@@ -3401,7 +3401,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>31</v>
       </c>
@@ -3430,7 +3430,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>41</v>
       </c>
@@ -3459,7 +3459,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>32</v>
       </c>
@@ -3489,7 +3489,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>46</v>
       </c>
@@ -3506,7 +3506,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>58</v>
       </c>
@@ -3538,19 +3538,19 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>64</v>
       </c>
@@ -3566,22 +3566,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4C4ABC5-F59E-4FB8-90DF-972E68413E6A}">
   <dimension ref="A1:P16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J16" sqref="J16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="61.375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="61.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="8.5" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="18.875" customWidth="1"/>
+    <col min="10" max="10" width="18.83203125" customWidth="1"/>
     <col min="11" max="11" width="14" customWidth="1"/>
     <col min="12" max="12" width="9" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="13.875" customWidth="1"/>
+    <col min="14" max="14" width="13.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1" s="29" t="s">
         <v>35</v>
       </c>
@@ -3601,7 +3601,7 @@
       <c r="M1" s="29"/>
       <c r="N1" s="29"/>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>54</v>
       </c>
@@ -3642,9 +3642,9 @@
       </c>
       <c r="P2" s="26"/>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
       <c r="C3" t="s">
         <v>81</v>
@@ -3662,9 +3662,9 @@
         <v>38</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
       <c r="C4" t="s">
         <v>66</v>
@@ -3682,9 +3682,9 @@
         <v>43</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
       <c r="C5" t="s">
         <v>65</v>
@@ -3702,9 +3702,9 @@
         <v>66</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
       <c r="C6" t="s">
         <v>69</v>
@@ -3728,9 +3728,9 @@
         <v>67</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
       <c r="C7" t="s">
         <v>70</v>
@@ -3757,9 +3757,9 @@
         <v>39</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
       <c r="C8" t="s">
         <v>71</v>
@@ -3786,9 +3786,9 @@
         <v>40</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
       <c r="C9" t="s">
         <v>76</v>
@@ -3815,9 +3815,9 @@
         <v>39</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
       <c r="C10" t="s">
         <v>76</v>
@@ -3844,9 +3844,9 @@
         <v>40</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
       <c r="C11" t="s">
         <v>59</v>
@@ -3870,9 +3870,9 @@
         <v>39</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
       <c r="C12" t="s">
         <v>72</v>
@@ -3899,9 +3899,9 @@
         <v>40</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
       <c r="C13" t="s">
         <v>73</v>
@@ -3925,9 +3925,9 @@
         <v>40</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
       <c r="C14" t="s">
         <v>74</v>
@@ -3942,9 +3942,9 @@
         <v>76</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
       <c r="C15" t="s">
         <v>75</v>
@@ -3953,9 +3953,9 @@
         <v>40</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
       <c r="C16" t="s">
         <v>76</v>
@@ -3982,9 +3982,9 @@
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>87</v>
       </c>
@@ -3992,7 +3992,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>89</v>
       </c>
@@ -4022,13 +4022,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4788DB3C-D649-48F4-9499-B599CC244B2F}">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>92</v>
       </c>
@@ -4039,7 +4039,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>96</v>
       </c>
@@ -4050,7 +4050,7 @@
         <v>1200</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>97</v>
       </c>
@@ -4073,7 +4073,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>